<commit_message>
Entrega PDF y documentos excel, donde se registran las evidencias
</commit_message>
<xml_diff>
--- a/1. Documentación/Matriz de riesgo.xlsx
+++ b/1. Documentación/Matriz de riesgo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10. SOFKAU\2. Programación\3. QA\C1-2023-QA-Calidad-RF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10. SOFKAU\2. Programación\3. QA\C1-2023-QA-Calidad-RF\1. Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4706562-1CAD-41F5-8998-A60AA614A039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178C3D82-0C50-4204-9587-73C955ED19FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,17 +896,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -919,37 +908,40 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -964,9 +956,17 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1683,87 +1683,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9940F568-0AEC-47A2-B308-46DDC97109A9}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="P32" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="25" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="25" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="25"/>
-    <col min="5" max="5" width="15.28515625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="11" style="25" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="25"/>
-    <col min="10" max="10" width="17.7109375" style="25" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="14" style="20" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="20" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="20"/>
+    <col min="5" max="5" width="15.28515625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="11" style="20" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="20"/>
+    <col min="10" max="10" width="17.7109375" style="20" customWidth="1"/>
+    <col min="11" max="12" width="0" style="20" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="20"/>
+    <col min="15" max="16" width="0" style="20" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24" t="s">
+      <c r="J1" s="39"/>
+      <c r="K1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24" t="s">
+      <c r="L1" s="39"/>
+      <c r="M1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24" t="s">
+      <c r="N1" s="39"/>
+      <c r="O1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="24"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="21">
         <v>1</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="21">
         <v>11</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="22">
         <v>11</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="28" t="s">
@@ -1784,70 +1787,70 @@
       <c r="P2" s="28"/>
     </row>
     <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="23">
         <v>1</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="23">
         <v>4</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="24">
         <v>4</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31" t="s">
+      <c r="J3" s="26"/>
+      <c r="K3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31" t="s">
+      <c r="L3" s="26"/>
+      <c r="M3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31" t="s">
+      <c r="N3" s="26"/>
+      <c r="O3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="31"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="21">
         <v>2</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="21">
         <v>2</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="24">
         <v>4</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="28" t="s">
@@ -1868,70 +1871,70 @@
       <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="23">
         <v>20</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="25">
         <v>20</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31" t="s">
+      <c r="J5" s="26"/>
+      <c r="K5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31" t="s">
+      <c r="L5" s="26"/>
+      <c r="M5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31" t="s">
+      <c r="N5" s="26"/>
+      <c r="O5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="31"/>
+      <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:16" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="21">
         <v>1</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="21">
         <v>5</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="24">
         <v>5</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="28" t="s">
@@ -1952,70 +1955,70 @@
       <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="23">
         <v>1</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="23">
         <v>10</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="24">
         <v>10</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="43" t="s">
+      <c r="J7" s="26"/>
+      <c r="K7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43" t="s">
+      <c r="L7" s="32"/>
+      <c r="M7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="43"/>
-      <c r="O7" s="39" t="s">
+      <c r="N7" s="32"/>
+      <c r="O7" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="40"/>
+      <c r="P7" s="36"/>
     </row>
     <row r="8" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="21">
         <v>1</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="21">
         <v>7</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="24">
         <v>7</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="28" t="s">
@@ -2030,76 +2033,76 @@
         <v>19</v>
       </c>
       <c r="N8" s="28"/>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="34"/>
+      <c r="P8" s="33"/>
     </row>
     <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="23">
         <v>1</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="23">
         <v>5</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="24">
         <v>5</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="43" t="s">
+      <c r="J9" s="26"/>
+      <c r="K9" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43" t="s">
+      <c r="L9" s="32"/>
+      <c r="M9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="43"/>
-      <c r="O9" s="33" t="s">
+      <c r="N9" s="32"/>
+      <c r="O9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="33"/>
+      <c r="P9" s="31"/>
     </row>
     <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="26">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="21">
         <v>1</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="21">
         <v>5</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="24">
         <v>5</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="28" t="s">
@@ -2114,76 +2117,76 @@
         <v>19</v>
       </c>
       <c r="N10" s="28"/>
-      <c r="O10" s="34" t="s">
+      <c r="O10" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="P10" s="34"/>
+      <c r="P10" s="33"/>
     </row>
     <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="23">
         <v>1</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="23">
         <v>5</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="24">
         <v>5</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="43" t="s">
+      <c r="J11" s="26"/>
+      <c r="K11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43" t="s">
+      <c r="L11" s="32"/>
+      <c r="M11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="43"/>
-      <c r="O11" s="33" t="s">
+      <c r="N11" s="32"/>
+      <c r="O11" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="P11" s="33"/>
+      <c r="P11" s="31"/>
     </row>
     <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="26">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="21">
         <v>1</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="21">
         <v>5</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="24">
         <v>5</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="28" t="s">
@@ -2198,76 +2201,76 @@
         <v>19</v>
       </c>
       <c r="N12" s="28"/>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="P12" s="34"/>
+      <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="23">
         <v>1</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="23">
         <v>2</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="24">
         <v>2</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="43" t="s">
+      <c r="J13" s="26"/>
+      <c r="K13" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43" t="s">
+      <c r="L13" s="32"/>
+      <c r="M13" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="43"/>
-      <c r="O13" s="33" t="s">
+      <c r="N13" s="32"/>
+      <c r="O13" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="P13" s="33"/>
+      <c r="P13" s="31"/>
     </row>
     <row r="14" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="26">
+      <c r="A14" s="21">
         <v>13</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="21">
         <v>1</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="21">
         <v>2</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="24">
         <v>2</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="28" t="s">
@@ -2282,76 +2285,76 @@
         <v>19</v>
       </c>
       <c r="N14" s="28"/>
-      <c r="O14" s="34" t="s">
+      <c r="O14" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="P14" s="34"/>
+      <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
+      <c r="A15" s="23">
         <v>14</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="23">
         <v>1</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="23">
         <v>5</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="24">
         <v>5</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="J15" s="31"/>
-      <c r="K15" s="43" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43" t="s">
+      <c r="L15" s="32"/>
+      <c r="M15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="33" t="s">
+      <c r="N15" s="32"/>
+      <c r="O15" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P15" s="33"/>
+      <c r="P15" s="31"/>
     </row>
     <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="26">
+      <c r="A16" s="21">
         <v>15</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="21">
         <v>4</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="21">
         <v>6</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="25">
         <v>24</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="28" t="s">
@@ -2366,496 +2369,496 @@
         <v>19</v>
       </c>
       <c r="N16" s="28"/>
-      <c r="O16" s="34" t="s">
+      <c r="O16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="P16" s="34"/>
+      <c r="P16" s="33"/>
     </row>
     <row r="17" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
+      <c r="A17" s="23">
         <v>16</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="23">
         <v>3</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="23">
         <v>5</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="22">
         <v>15</v>
       </c>
-      <c r="H17" s="29" t="s">
+      <c r="H17" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="43" t="s">
+      <c r="J17" s="26"/>
+      <c r="K17" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43" t="s">
+      <c r="L17" s="32"/>
+      <c r="M17" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="43"/>
-      <c r="O17" s="33" t="s">
+      <c r="N17" s="32"/>
+      <c r="O17" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="P17" s="33"/>
+      <c r="P17" s="31"/>
     </row>
     <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="21">
         <v>17</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="21">
         <v>4</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="21">
         <v>5</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="25">
         <v>20</v>
       </c>
-      <c r="H18" s="26" t="s">
+      <c r="H18" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I18" s="28" t="s">
         <v>140</v>
       </c>
       <c r="J18" s="28"/>
-      <c r="K18" s="41" t="s">
+      <c r="K18" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="L18" s="42"/>
+      <c r="L18" s="38"/>
       <c r="M18" s="28" t="s">
         <v>19</v>
       </c>
       <c r="N18" s="28"/>
-      <c r="O18" s="34" t="s">
+      <c r="O18" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="P18" s="34"/>
+      <c r="P18" s="33"/>
     </row>
     <row r="19" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="A19" s="23">
         <v>18</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="23">
         <v>3</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="23">
         <v>5</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="22">
         <v>15</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="39" t="s">
+      <c r="J19" s="26"/>
+      <c r="K19" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="40"/>
-      <c r="M19" s="43" t="s">
+      <c r="L19" s="36"/>
+      <c r="M19" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N19" s="43"/>
-      <c r="O19" s="33" t="s">
+      <c r="N19" s="32"/>
+      <c r="O19" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P19" s="33"/>
+      <c r="P19" s="31"/>
     </row>
     <row r="20" spans="1:16" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26">
+      <c r="A20" s="21">
         <v>19</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="21">
         <v>3</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="21">
         <v>2</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="24">
         <v>6</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I20" s="28" t="s">
         <v>142</v>
       </c>
       <c r="J20" s="28"/>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="34"/>
+      <c r="L20" s="33"/>
       <c r="M20" s="28" t="s">
         <v>19</v>
       </c>
       <c r="N20" s="28"/>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="P20" s="34"/>
+      <c r="P20" s="33"/>
     </row>
     <row r="21" spans="1:16" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="23">
         <v>20</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="23">
         <v>1</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="23">
         <v>3</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="24">
         <v>3</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="35" t="s">
+      <c r="J21" s="26"/>
+      <c r="K21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="35"/>
-      <c r="M21" s="43" t="s">
+      <c r="L21" s="34"/>
+      <c r="M21" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="43"/>
-      <c r="O21" s="35" t="s">
+      <c r="N21" s="32"/>
+      <c r="O21" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="P21" s="35"/>
+      <c r="P21" s="34"/>
     </row>
     <row r="22" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="26">
+      <c r="A22" s="21">
         <v>21</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="21">
         <v>2</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="21">
         <v>7</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="22">
         <v>14</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="H22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I22" s="28" t="s">
         <v>144</v>
       </c>
       <c r="J22" s="28"/>
-      <c r="K22" s="34" t="s">
+      <c r="K22" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="L22" s="34"/>
+      <c r="L22" s="33"/>
       <c r="M22" s="28" t="s">
         <v>16</v>
       </c>
       <c r="N22" s="28"/>
-      <c r="O22" s="34" t="s">
+      <c r="O22" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="P22" s="34"/>
+      <c r="P22" s="33"/>
     </row>
     <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
+      <c r="A23" s="23">
         <v>22</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="23">
         <v>1</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="23">
         <v>4</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="24">
         <v>4</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="J23" s="31"/>
-      <c r="K23" s="33" t="s">
+      <c r="J23" s="26"/>
+      <c r="K23" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="L23" s="33"/>
-      <c r="M23" s="43" t="s">
+      <c r="L23" s="31"/>
+      <c r="M23" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N23" s="43"/>
-      <c r="O23" s="33" t="s">
+      <c r="N23" s="32"/>
+      <c r="O23" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="P23" s="33"/>
+      <c r="P23" s="31"/>
     </row>
     <row r="24" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="26">
+      <c r="A24" s="21">
         <v>23</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="21">
         <v>3</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="21">
         <v>5</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="22">
         <v>15</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="21" t="s">
         <v>124</v>
       </c>
       <c r="I24" s="28" t="s">
         <v>146</v>
       </c>
       <c r="J24" s="28"/>
-      <c r="K24" s="34" t="s">
+      <c r="K24" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="L24" s="34"/>
+      <c r="L24" s="33"/>
       <c r="M24" s="28" t="s">
         <v>16</v>
       </c>
       <c r="N24" s="28"/>
-      <c r="O24" s="34" t="s">
+      <c r="O24" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="P24" s="34"/>
+      <c r="P24" s="33"/>
     </row>
     <row r="25" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="A25" s="23">
         <v>24</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="23">
         <v>2</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="23">
         <v>6</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="22">
         <v>12</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="31" t="s">
+      <c r="I25" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="J25" s="31"/>
-      <c r="K25" s="33" t="s">
+      <c r="J25" s="26"/>
+      <c r="K25" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="L25" s="33"/>
-      <c r="M25" s="43" t="s">
+      <c r="L25" s="31"/>
+      <c r="M25" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="N25" s="43"/>
-      <c r="O25" s="33" t="s">
+      <c r="N25" s="32"/>
+      <c r="O25" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P25" s="33"/>
+      <c r="P25" s="31"/>
     </row>
     <row r="26" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26">
+      <c r="A26" s="21">
         <v>25</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="21">
         <v>2</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="21">
         <v>2</v>
       </c>
-      <c r="G26" s="30">
+      <c r="G26" s="24">
         <v>4</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="H26" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36" t="s">
+      <c r="J26" s="27"/>
+      <c r="K26" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L26" s="36"/>
+      <c r="L26" s="27"/>
       <c r="M26" s="28" t="s">
         <v>19</v>
       </c>
       <c r="N26" s="28"/>
-      <c r="O26" s="37" t="s">
+      <c r="O26" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="P26" s="38"/>
+      <c r="P26" s="30"/>
     </row>
     <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
+      <c r="A27" s="23">
         <v>26</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="23">
         <v>2</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="23">
         <v>5</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="24">
         <v>10</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="H27" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="31" t="s">
+      <c r="I27" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31" t="s">
+      <c r="J27" s="26"/>
+      <c r="K27" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31" t="s">
+      <c r="L27" s="26"/>
+      <c r="M27" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31" t="s">
+      <c r="N27" s="26"/>
+      <c r="O27" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="P27" s="31"/>
+      <c r="P27" s="26"/>
     </row>
     <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="26">
+      <c r="A28" s="21">
         <v>27</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="21">
         <v>2</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="21">
         <v>10</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="25">
         <v>20</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I28" s="28" t="s">
@@ -2876,70 +2879,70 @@
       <c r="P28" s="28"/>
     </row>
     <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
+      <c r="A29" s="23">
         <v>28</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="23">
         <v>2</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="23">
         <v>10</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="25">
         <v>20</v>
       </c>
-      <c r="H29" s="29" t="s">
+      <c r="H29" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="31" t="s">
+      <c r="I29" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31" t="s">
+      <c r="J29" s="26"/>
+      <c r="K29" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31" t="s">
+      <c r="L29" s="26"/>
+      <c r="M29" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31" t="s">
+      <c r="N29" s="26"/>
+      <c r="O29" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="P29" s="31"/>
+      <c r="P29" s="26"/>
     </row>
     <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="26">
+      <c r="A30" s="21">
         <v>29</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E30" s="21">
         <v>2</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F30" s="21">
         <v>10</v>
       </c>
-      <c r="G30" s="32">
+      <c r="G30" s="25">
         <v>20</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="H30" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I30" s="28" t="s">
@@ -2960,49 +2963,149 @@
       <c r="P30" s="28"/>
     </row>
     <row r="31" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
+      <c r="A31" s="23">
         <v>30</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="23">
         <v>1</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="23">
         <v>3</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="24">
         <v>3</v>
       </c>
-      <c r="H31" s="29" t="s">
+      <c r="H31" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="31" t="s">
+      <c r="I31" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31" t="s">
+      <c r="J31" s="26"/>
+      <c r="K31" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31" t="s">
+      <c r="L31" s="26"/>
+      <c r="M31" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31" t="s">
+      <c r="N31" s="26"/>
+      <c r="O31" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="P31" s="31"/>
+      <c r="P31" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="M31:N31"/>
@@ -3027,106 +3130,6 @@
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="O28:P28"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3186,10 +3189,10 @@
       <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="20"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4423,10 +4426,10 @@
       <c r="G1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="22"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="8" t="s">
         <v>77</v>
       </c>

</xml_diff>